<commit_message>
Fix Mapping to ISO27001:2022
</commit_message>
<xml_diff>
--- a/tools/excel/NIS2/mappings/mapping-annex-technical-and-methodological-requirements-nis2-and-iso27001-2022.xlsx
+++ b/tools/excel/NIS2/mappings/mapping-annex-technical-and-methodological-requirements-nis2-and-iso27001-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\NIS2\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D06979-7EA1-4F78-B6A2-7B4AE837DFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2093545C-DCE5-4B1F-BC50-65854855D122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="-15750" windowWidth="12810" windowHeight="15855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2145" yWindow="-13470" windowWidth="21795" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="source" sheetId="5" r:id="rId5"/>
     <sheet name="target" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5262" uniqueCount="1955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5265" uniqueCount="1956">
   <si>
     <t>type</t>
   </si>
@@ -5890,6 +5890,9 @@
   </si>
   <si>
     <t>Annex-to-the-Implementing-Regulation-of-NIS2-on-Technical-and-methodological-requirements &lt;-&gt; ISO/IEC 27001:2022</t>
+  </si>
+  <si>
+    <t>EUROPEAN COMMISSION</t>
   </si>
 </sst>
 </file>
@@ -5925,7 +5928,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -6232,8 +6237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6303,7 +6308,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6311,7 +6316,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -6339,7 +6344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -6428,11 +6433,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E954"/>
+  <dimension ref="A1:E955"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A703" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D714" sqref="D714"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14226,8 +14231,8 @@
       </c>
     </row>
     <row r="708" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A708" s="1" t="s">
-        <v>173</v>
+      <c r="A708" t="s">
+        <v>236</v>
       </c>
       <c r="B708" s="1" t="s">
         <v>1817</v>
@@ -14237,8 +14242,8 @@
       </c>
     </row>
     <row r="709" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A709" s="1" t="s">
-        <v>174</v>
+      <c r="A709" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="B709" s="1" t="s">
         <v>1817</v>
@@ -14248,8 +14253,8 @@
       </c>
     </row>
     <row r="710" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A710" s="1" t="s">
-        <v>175</v>
+      <c r="A710" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="B710" s="1" t="s">
         <v>1817</v>
@@ -14259,8 +14264,8 @@
       </c>
     </row>
     <row r="711" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A711" s="1" t="s">
-        <v>176</v>
+      <c r="A711" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="B711" s="1" t="s">
         <v>1817</v>
@@ -14270,8 +14275,8 @@
       </c>
     </row>
     <row r="712" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A712" s="1" t="s">
-        <v>177</v>
+      <c r="A712" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="B712" s="1" t="s">
         <v>1817</v>
@@ -14281,8 +14286,8 @@
       </c>
     </row>
     <row r="713" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A713" s="1" t="s">
-        <v>178</v>
+      <c r="A713" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="B713" s="1" t="s">
         <v>1817</v>
@@ -14291,20 +14296,20 @@
         <v>383</v>
       </c>
     </row>
-    <row r="714" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A714" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B714" s="1" t="s">
+    <row r="714" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A714" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B714" s="3" t="s">
         <v>1817</v>
       </c>
-      <c r="C714" t="s">
+      <c r="C714" s="2" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="715" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A715" s="1" t="s">
-        <v>180</v>
+      <c r="A715" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="B715" s="1" t="s">
         <v>1817</v>
@@ -14314,11 +14319,11 @@
       </c>
     </row>
     <row r="716" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A716" t="s">
-        <v>244</v>
-      </c>
-      <c r="B716" t="s">
-        <v>787</v>
+      <c r="A716" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B716" s="1" t="s">
+        <v>1817</v>
       </c>
       <c r="C716" t="s">
         <v>383</v>
@@ -14329,18 +14334,18 @@
         <v>244</v>
       </c>
       <c r="B717" t="s">
+        <v>787</v>
+      </c>
+      <c r="C717" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="718" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A718" t="s">
+        <v>244</v>
+      </c>
+      <c r="B718" t="s">
         <v>267</v>
-      </c>
-      <c r="C717" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="718" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A718" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B718" s="1" t="s">
-        <v>1455</v>
       </c>
       <c r="C718" t="s">
         <v>383</v>
@@ -14351,7 +14356,7 @@
         <v>244</v>
       </c>
       <c r="B719" s="1" t="s">
-        <v>1458</v>
+        <v>1455</v>
       </c>
       <c r="C719" t="s">
         <v>383</v>
@@ -14362,7 +14367,7 @@
         <v>244</v>
       </c>
       <c r="B720" s="1" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
       <c r="C720" t="s">
         <v>383</v>
@@ -14370,10 +14375,10 @@
     </row>
     <row r="721" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A721" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B721" s="1" t="s">
-        <v>252</v>
+        <v>1462</v>
       </c>
       <c r="C721" t="s">
         <v>383</v>
@@ -14381,7 +14386,7 @@
     </row>
     <row r="722" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A722" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B722" s="1" t="s">
         <v>252</v>
@@ -14392,7 +14397,7 @@
     </row>
     <row r="723" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A723" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B723" s="1" t="s">
         <v>252</v>
@@ -14403,7 +14408,7 @@
     </row>
     <row r="724" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A724" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B724" s="1" t="s">
         <v>252</v>
@@ -14414,7 +14419,7 @@
     </row>
     <row r="725" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A725" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B725" s="1" t="s">
         <v>252</v>
@@ -14425,7 +14430,7 @@
     </row>
     <row r="726" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A726" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B726" s="1" t="s">
         <v>252</v>
@@ -14436,10 +14441,10 @@
     </row>
     <row r="727" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A727" s="1" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B727" s="1" t="s">
-        <v>1678</v>
+        <v>252</v>
       </c>
       <c r="C727" t="s">
         <v>383</v>
@@ -14447,7 +14452,7 @@
     </row>
     <row r="728" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A728" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B728" s="1" t="s">
         <v>1678</v>
@@ -14458,7 +14463,7 @@
     </row>
     <row r="729" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A729" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B729" s="1" t="s">
         <v>1678</v>
@@ -14469,7 +14474,7 @@
     </row>
     <row r="730" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A730" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B730" s="1" t="s">
         <v>1678</v>
@@ -14480,7 +14485,7 @@
     </row>
     <row r="731" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A731" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B731" s="1" t="s">
         <v>1678</v>
@@ -14491,7 +14496,7 @@
     </row>
     <row r="732" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A732" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B732" s="1" t="s">
         <v>1678</v>
@@ -14502,10 +14507,10 @@
     </row>
     <row r="733" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A733" s="1" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B733" s="1" t="s">
-        <v>1812</v>
+        <v>1678</v>
       </c>
       <c r="C733" t="s">
         <v>383</v>
@@ -14513,7 +14518,7 @@
     </row>
     <row r="734" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A734" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B734" s="1" t="s">
         <v>1812</v>
@@ -14524,7 +14529,7 @@
     </row>
     <row r="735" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A735" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B735" s="1" t="s">
         <v>1812</v>
@@ -14535,7 +14540,7 @@
     </row>
     <row r="736" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A736" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B736" s="1" t="s">
         <v>1812</v>
@@ -14546,7 +14551,7 @@
     </row>
     <row r="737" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A737" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B737" s="1" t="s">
         <v>1812</v>
@@ -14557,7 +14562,7 @@
     </row>
     <row r="738" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A738" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B738" s="1" t="s">
         <v>1812</v>
@@ -14568,10 +14573,10 @@
     </row>
     <row r="739" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A739" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B739" s="1" t="s">
-        <v>245</v>
+        <v>1812</v>
       </c>
       <c r="C739" t="s">
         <v>383</v>
@@ -14579,7 +14584,7 @@
     </row>
     <row r="740" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A740" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B740" s="1" t="s">
         <v>245</v>
@@ -14590,7 +14595,7 @@
     </row>
     <row r="741" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A741" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B741" s="1" t="s">
         <v>245</v>
@@ -14601,7 +14606,7 @@
     </row>
     <row r="742" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A742" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B742" s="1" t="s">
         <v>245</v>
@@ -14612,7 +14617,7 @@
     </row>
     <row r="743" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A743" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B743" s="1" t="s">
         <v>245</v>
@@ -14623,7 +14628,7 @@
     </row>
     <row r="744" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A744" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B744" s="1" t="s">
         <v>245</v>
@@ -14634,7 +14639,7 @@
     </row>
     <row r="745" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A745" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B745" s="1" t="s">
         <v>245</v>
@@ -14645,7 +14650,7 @@
     </row>
     <row r="746" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A746" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B746" s="1" t="s">
         <v>245</v>
@@ -14656,10 +14661,10 @@
     </row>
     <row r="747" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A747" s="1" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="B747" s="1" t="s">
-        <v>1678</v>
+        <v>245</v>
       </c>
       <c r="C747" t="s">
         <v>383</v>
@@ -14667,7 +14672,7 @@
     </row>
     <row r="748" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A748" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B748" s="1" t="s">
         <v>1678</v>
@@ -14678,7 +14683,7 @@
     </row>
     <row r="749" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A749" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B749" s="1" t="s">
         <v>1678</v>
@@ -14689,7 +14694,7 @@
     </row>
     <row r="750" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A750" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B750" s="1" t="s">
         <v>1678</v>
@@ -14700,7 +14705,7 @@
     </row>
     <row r="751" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A751" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B751" s="1" t="s">
         <v>1678</v>
@@ -14711,7 +14716,7 @@
     </row>
     <row r="752" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A752" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B752" s="1" t="s">
         <v>1678</v>
@@ -14722,7 +14727,7 @@
     </row>
     <row r="753" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A753" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B753" s="1" t="s">
         <v>1678</v>
@@ -14733,7 +14738,7 @@
     </row>
     <row r="754" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A754" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B754" s="1" t="s">
         <v>1678</v>
@@ -14743,11 +14748,11 @@
       </c>
     </row>
     <row r="755" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A755" t="s">
-        <v>267</v>
-      </c>
-      <c r="B755" t="s">
-        <v>1630</v>
+      <c r="A755" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B755" s="1" t="s">
+        <v>1678</v>
       </c>
       <c r="C755" t="s">
         <v>383</v>
@@ -14758,18 +14763,18 @@
         <v>267</v>
       </c>
       <c r="B756" t="s">
+        <v>1630</v>
+      </c>
+      <c r="C756" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="757" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A757" t="s">
+        <v>267</v>
+      </c>
+      <c r="B757" t="s">
         <v>1896</v>
-      </c>
-      <c r="C756" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="757" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A757" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="B757" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="C757" t="s">
         <v>383</v>
@@ -14777,7 +14782,7 @@
     </row>
     <row r="758" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A758" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B758" s="1" t="s">
         <v>244</v>
@@ -14788,7 +14793,7 @@
     </row>
     <row r="759" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A759" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B759" s="1" t="s">
         <v>244</v>
@@ -14799,7 +14804,7 @@
     </row>
     <row r="760" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A760" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B760" s="1" t="s">
         <v>244</v>
@@ -14810,7 +14815,7 @@
     </row>
     <row r="761" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A761" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B761" s="1" t="s">
         <v>244</v>
@@ -14821,7 +14826,7 @@
     </row>
     <row r="762" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A762" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B762" s="1" t="s">
         <v>244</v>
@@ -14832,10 +14837,10 @@
     </row>
     <row r="763" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A763" s="1" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="B763" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C763" t="s">
         <v>383</v>
@@ -14843,7 +14848,7 @@
     </row>
     <row r="764" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A764" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B764" s="1" t="s">
         <v>245</v>
@@ -14854,7 +14859,7 @@
     </row>
     <row r="765" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A765" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B765" s="1" t="s">
         <v>245</v>
@@ -14865,7 +14870,7 @@
     </row>
     <row r="766" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A766" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B766" s="1" t="s">
         <v>245</v>
@@ -14876,7 +14881,7 @@
     </row>
     <row r="767" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A767" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B767" s="1" t="s">
         <v>245</v>
@@ -14887,7 +14892,7 @@
     </row>
     <row r="768" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A768" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B768" s="1" t="s">
         <v>245</v>
@@ -14898,10 +14903,10 @@
     </row>
     <row r="769" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A769" s="1" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="B769" s="1" t="s">
-        <v>1673</v>
+        <v>245</v>
       </c>
       <c r="C769" t="s">
         <v>383</v>
@@ -14909,7 +14914,7 @@
     </row>
     <row r="770" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A770" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B770" s="1" t="s">
         <v>1673</v>
@@ -14920,7 +14925,7 @@
     </row>
     <row r="771" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A771" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B771" s="1" t="s">
         <v>1673</v>
@@ -14931,7 +14936,7 @@
     </row>
     <row r="772" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A772" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B772" s="1" t="s">
         <v>1673</v>
@@ -14942,7 +14947,7 @@
     </row>
     <row r="773" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A773" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B773" s="1" t="s">
         <v>1673</v>
@@ -14953,7 +14958,7 @@
     </row>
     <row r="774" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A774" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B774" s="1" t="s">
         <v>1673</v>
@@ -14964,10 +14969,10 @@
     </row>
     <row r="775" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A775" s="1" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="B775" s="1" t="s">
-        <v>1678</v>
+        <v>1673</v>
       </c>
       <c r="C775" t="s">
         <v>383</v>
@@ -14975,7 +14980,7 @@
     </row>
     <row r="776" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A776" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B776" s="1" t="s">
         <v>1678</v>
@@ -14986,7 +14991,7 @@
     </row>
     <row r="777" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A777" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B777" s="1" t="s">
         <v>1678</v>
@@ -14997,7 +15002,7 @@
     </row>
     <row r="778" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A778" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B778" s="1" t="s">
         <v>1678</v>
@@ -15008,7 +15013,7 @@
     </row>
     <row r="779" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A779" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B779" s="1" t="s">
         <v>1678</v>
@@ -15019,7 +15024,7 @@
     </row>
     <row r="780" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A780" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B780" s="1" t="s">
         <v>1678</v>
@@ -15030,10 +15035,10 @@
     </row>
     <row r="781" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A781" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B781" s="1" t="s">
-        <v>1668</v>
+        <v>1678</v>
       </c>
       <c r="C781" t="s">
         <v>383</v>
@@ -15041,7 +15046,7 @@
     </row>
     <row r="782" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A782" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B782" s="1" t="s">
         <v>1668</v>
@@ -15052,7 +15057,7 @@
     </row>
     <row r="783" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A783" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B783" s="1" t="s">
         <v>1668</v>
@@ -15063,7 +15068,7 @@
     </row>
     <row r="784" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A784" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B784" s="1" t="s">
         <v>1668</v>
@@ -15074,10 +15079,10 @@
     </row>
     <row r="785" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A785" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B785" s="1" t="s">
-        <v>1687</v>
+        <v>1668</v>
       </c>
       <c r="C785" t="s">
         <v>383</v>
@@ -15085,7 +15090,7 @@
     </row>
     <row r="786" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A786" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B786" s="1" t="s">
         <v>1687</v>
@@ -15096,10 +15101,10 @@
     </row>
     <row r="787" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A787" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B787" s="1" t="s">
-        <v>1615</v>
+        <v>1687</v>
       </c>
       <c r="C787" t="s">
         <v>383</v>
@@ -15107,7 +15112,7 @@
     </row>
     <row r="788" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A788" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B788" s="1" t="s">
         <v>1615</v>
@@ -15118,10 +15123,10 @@
     </row>
     <row r="789" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A789" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B789" s="1" t="s">
-        <v>1683</v>
+        <v>1615</v>
       </c>
       <c r="C789" t="s">
         <v>383</v>
@@ -15129,7 +15134,7 @@
     </row>
     <row r="790" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A790" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B790" s="1" t="s">
         <v>1683</v>
@@ -15140,10 +15145,10 @@
     </row>
     <row r="791" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A791" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B791" s="1" t="s">
-        <v>1550</v>
+        <v>1683</v>
       </c>
       <c r="C791" t="s">
         <v>383</v>
@@ -15151,7 +15156,7 @@
     </row>
     <row r="792" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A792" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B792" s="1" t="s">
         <v>1550</v>
@@ -15162,7 +15167,7 @@
     </row>
     <row r="793" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A793" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B793" s="1" t="s">
         <v>1550</v>
@@ -15173,7 +15178,7 @@
     </row>
     <row r="794" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A794" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B794" s="1" t="s">
         <v>1550</v>
@@ -15184,7 +15189,7 @@
     </row>
     <row r="795" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A795" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B795" s="1" t="s">
         <v>1550</v>
@@ -15195,10 +15200,10 @@
     </row>
     <row r="796" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A796" s="1" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>1715</v>
+        <v>1550</v>
       </c>
       <c r="C796" t="s">
         <v>383</v>
@@ -15206,7 +15211,7 @@
     </row>
     <row r="797" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A797" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B797" s="1" t="s">
         <v>1715</v>
@@ -15217,7 +15222,7 @@
     </row>
     <row r="798" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A798" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B798" s="1" t="s">
         <v>1715</v>
@@ -15228,7 +15233,7 @@
     </row>
     <row r="799" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A799" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B799" s="1" t="s">
         <v>1715</v>
@@ -15239,7 +15244,7 @@
     </row>
     <row r="800" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A800" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B800" s="1" t="s">
         <v>1715</v>
@@ -15250,10 +15255,10 @@
     </row>
     <row r="801" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A801" s="1" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B801" s="1" t="s">
-        <v>1792</v>
+        <v>1715</v>
       </c>
       <c r="C801" t="s">
         <v>383</v>
@@ -15261,7 +15266,7 @@
     </row>
     <row r="802" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A802" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B802" s="1" t="s">
         <v>1792</v>
@@ -15272,7 +15277,7 @@
     </row>
     <row r="803" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A803" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B803" s="1" t="s">
         <v>1792</v>
@@ -15283,7 +15288,7 @@
     </row>
     <row r="804" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A804" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B804" s="1" t="s">
         <v>1792</v>
@@ -15294,7 +15299,7 @@
     </row>
     <row r="805" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A805" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B805" s="1" t="s">
         <v>1792</v>
@@ -15305,10 +15310,10 @@
     </row>
     <row r="806" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A806" s="1" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>1881</v>
+        <v>1792</v>
       </c>
       <c r="C806" t="s">
         <v>383</v>
@@ -15316,7 +15321,7 @@
     </row>
     <row r="807" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A807" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B807" s="1" t="s">
         <v>1881</v>
@@ -15327,7 +15332,7 @@
     </row>
     <row r="808" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A808" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B808" s="1" t="s">
         <v>1881</v>
@@ -15338,7 +15343,7 @@
     </row>
     <row r="809" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A809" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B809" s="1" t="s">
         <v>1881</v>
@@ -15349,7 +15354,7 @@
     </row>
     <row r="810" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A810" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B810" s="1" t="s">
         <v>1881</v>
@@ -15360,10 +15365,10 @@
     </row>
     <row r="811" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A811" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B811" s="1" t="s">
-        <v>1490</v>
+        <v>1881</v>
       </c>
       <c r="C811" t="s">
         <v>383</v>
@@ -15371,7 +15376,7 @@
     </row>
     <row r="812" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A812" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B812" s="1" t="s">
         <v>1490</v>
@@ -15382,7 +15387,7 @@
     </row>
     <row r="813" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A813" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B813" s="1" t="s">
         <v>1490</v>
@@ -15393,7 +15398,7 @@
     </row>
     <row r="814" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A814" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B814" s="1" t="s">
         <v>1490</v>
@@ -15404,7 +15409,7 @@
     </row>
     <row r="815" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A815" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B815" s="1" t="s">
         <v>1490</v>
@@ -15415,7 +15420,7 @@
     </row>
     <row r="816" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A816" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B816" s="1" t="s">
         <v>1490</v>
@@ -15426,7 +15431,7 @@
     </row>
     <row r="817" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A817" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B817" s="1" t="s">
         <v>1490</v>
@@ -15437,7 +15442,7 @@
     </row>
     <row r="818" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A818" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B818" s="1" t="s">
         <v>1490</v>
@@ -15448,10 +15453,10 @@
     </row>
     <row r="819" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A819" s="1" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="B819" s="1" t="s">
-        <v>1565</v>
+        <v>1490</v>
       </c>
       <c r="C819" t="s">
         <v>383</v>
@@ -15459,7 +15464,7 @@
     </row>
     <row r="820" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A820" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B820" s="1" t="s">
         <v>1565</v>
@@ -15470,7 +15475,7 @@
     </row>
     <row r="821" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A821" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B821" s="1" t="s">
         <v>1565</v>
@@ -15481,7 +15486,7 @@
     </row>
     <row r="822" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A822" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B822" s="1" t="s">
         <v>1565</v>
@@ -15492,7 +15497,7 @@
     </row>
     <row r="823" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A823" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B823" s="1" t="s">
         <v>1565</v>
@@ -15503,7 +15508,7 @@
     </row>
     <row r="824" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A824" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B824" s="1" t="s">
         <v>1565</v>
@@ -15514,7 +15519,7 @@
     </row>
     <row r="825" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A825" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B825" s="1" t="s">
         <v>1565</v>
@@ -15525,7 +15530,7 @@
     </row>
     <row r="826" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A826" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B826" s="1" t="s">
         <v>1565</v>
@@ -15536,10 +15541,10 @@
     </row>
     <row r="827" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A827" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>1787</v>
+        <v>1565</v>
       </c>
       <c r="C827" t="s">
         <v>383</v>
@@ -15547,7 +15552,7 @@
     </row>
     <row r="828" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A828" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B828" s="1" t="s">
         <v>1787</v>
@@ -15558,7 +15563,7 @@
     </row>
     <row r="829" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A829" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B829" s="1" t="s">
         <v>1787</v>
@@ -15569,7 +15574,7 @@
     </row>
     <row r="830" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A830" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B830" s="1" t="s">
         <v>1787</v>
@@ -15580,7 +15585,7 @@
     </row>
     <row r="831" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A831" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B831" s="1" t="s">
         <v>1787</v>
@@ -15591,7 +15596,7 @@
     </row>
     <row r="832" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A832" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B832" s="1" t="s">
         <v>1787</v>
@@ -15602,10 +15607,10 @@
     </row>
     <row r="833" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A833" s="1" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="B833" s="1" t="s">
-        <v>1866</v>
+        <v>1787</v>
       </c>
       <c r="C833" t="s">
         <v>383</v>
@@ -15613,7 +15618,7 @@
     </row>
     <row r="834" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A834" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B834" s="1" t="s">
         <v>1866</v>
@@ -15624,7 +15629,7 @@
     </row>
     <row r="835" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A835" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B835" s="1" t="s">
         <v>1866</v>
@@ -15635,7 +15640,7 @@
     </row>
     <row r="836" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A836" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B836" s="1" t="s">
         <v>1866</v>
@@ -15646,7 +15651,7 @@
     </row>
     <row r="837" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A837" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B837" s="1" t="s">
         <v>1866</v>
@@ -15657,7 +15662,7 @@
     </row>
     <row r="838" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A838" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B838" s="1" t="s">
         <v>1866</v>
@@ -15668,10 +15673,10 @@
     </row>
     <row r="839" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A839" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B839" s="1" t="s">
-        <v>1787</v>
+        <v>1866</v>
       </c>
       <c r="C839" t="s">
         <v>383</v>
@@ -15679,7 +15684,7 @@
     </row>
     <row r="840" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A840" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B840" s="1" t="s">
         <v>1787</v>
@@ -15690,7 +15695,7 @@
     </row>
     <row r="841" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A841" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B841" s="1" t="s">
         <v>1787</v>
@@ -15701,7 +15706,7 @@
     </row>
     <row r="842" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A842" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B842" s="1" t="s">
         <v>1787</v>
@@ -15712,10 +15717,10 @@
     </row>
     <row r="843" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A843" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B843" s="1" t="s">
-        <v>1866</v>
+        <v>1787</v>
       </c>
       <c r="C843" t="s">
         <v>383</v>
@@ -15723,7 +15728,7 @@
     </row>
     <row r="844" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A844" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B844" s="1" t="s">
         <v>1866</v>
@@ -15734,7 +15739,7 @@
     </row>
     <row r="845" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A845" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B845" s="1" t="s">
         <v>1866</v>
@@ -15745,7 +15750,7 @@
     </row>
     <row r="846" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A846" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B846" s="1" t="s">
         <v>1866</v>
@@ -15756,10 +15761,10 @@
     </row>
     <row r="847" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A847" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B847" s="1" t="s">
-        <v>1555</v>
+        <v>1866</v>
       </c>
       <c r="C847" t="s">
         <v>383</v>
@@ -15767,7 +15772,7 @@
     </row>
     <row r="848" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A848" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B848" s="1" t="s">
         <v>1555</v>
@@ -15778,7 +15783,7 @@
     </row>
     <row r="849" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A849" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B849" s="1" t="s">
         <v>1555</v>
@@ -15789,7 +15794,7 @@
     </row>
     <row r="850" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A850" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B850" s="1" t="s">
         <v>1555</v>
@@ -15800,7 +15805,7 @@
     </row>
     <row r="851" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A851" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B851" s="1" t="s">
         <v>1555</v>
@@ -15811,7 +15816,7 @@
     </row>
     <row r="852" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A852" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B852" s="1" t="s">
         <v>1555</v>
@@ -15822,7 +15827,7 @@
     </row>
     <row r="853" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A853" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B853" s="1" t="s">
         <v>1555</v>
@@ -15833,10 +15838,10 @@
     </row>
     <row r="854" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A854" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>1560</v>
+        <v>1555</v>
       </c>
       <c r="C854" t="s">
         <v>383</v>
@@ -15844,7 +15849,7 @@
     </row>
     <row r="855" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A855" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B855" s="1" t="s">
         <v>1560</v>
@@ -15855,7 +15860,7 @@
     </row>
     <row r="856" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A856" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B856" s="1" t="s">
         <v>1560</v>
@@ -15866,7 +15871,7 @@
     </row>
     <row r="857" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A857" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B857" s="1" t="s">
         <v>1560</v>
@@ -15877,7 +15882,7 @@
     </row>
     <row r="858" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A858" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B858" s="1" t="s">
         <v>1560</v>
@@ -15888,7 +15893,7 @@
     </row>
     <row r="859" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A859" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B859" s="1" t="s">
         <v>1560</v>
@@ -15899,7 +15904,7 @@
     </row>
     <row r="860" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A860" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B860" s="1" t="s">
         <v>1560</v>
@@ -15910,7 +15915,7 @@
     </row>
     <row r="861" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A861" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B861" s="1" t="s">
         <v>1560</v>
@@ -15921,7 +15926,7 @@
     </row>
     <row r="862" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A862" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B862" s="1" t="s">
         <v>1560</v>
@@ -15932,10 +15937,10 @@
     </row>
     <row r="863" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A863" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B863" s="1" t="s">
-        <v>1802</v>
+        <v>1560</v>
       </c>
       <c r="C863" t="s">
         <v>383</v>
@@ -15943,7 +15948,7 @@
     </row>
     <row r="864" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A864" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B864" s="1" t="s">
         <v>1802</v>
@@ -15954,10 +15959,10 @@
     </row>
     <row r="865" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A865" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B865" s="1" t="s">
-        <v>1520</v>
+        <v>1802</v>
       </c>
       <c r="C865" t="s">
         <v>383</v>
@@ -15965,7 +15970,7 @@
     </row>
     <row r="866" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A866" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B866" s="1" t="s">
         <v>1520</v>
@@ -15976,7 +15981,7 @@
     </row>
     <row r="867" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A867" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B867" s="1" t="s">
         <v>1520</v>
@@ -15987,7 +15992,7 @@
     </row>
     <row r="868" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A868" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B868" s="1" t="s">
         <v>1520</v>
@@ -15998,7 +16003,7 @@
     </row>
     <row r="869" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A869" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B869" s="1" t="s">
         <v>1520</v>
@@ -16009,10 +16014,10 @@
     </row>
     <row r="870" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A870" s="1" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B870" s="1" t="s">
-        <v>1535</v>
+        <v>1520</v>
       </c>
       <c r="C870" t="s">
         <v>383</v>
@@ -16020,7 +16025,7 @@
     </row>
     <row r="871" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A871" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B871" s="1" t="s">
         <v>1535</v>
@@ -16031,7 +16036,7 @@
     </row>
     <row r="872" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A872" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B872" s="1" t="s">
         <v>1535</v>
@@ -16042,7 +16047,7 @@
     </row>
     <row r="873" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A873" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B873" s="1" t="s">
         <v>1535</v>
@@ -16053,7 +16058,7 @@
     </row>
     <row r="874" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A874" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B874" s="1" t="s">
         <v>1535</v>
@@ -16064,10 +16069,10 @@
     </row>
     <row r="875" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A875" s="1" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>1540</v>
+        <v>1535</v>
       </c>
       <c r="C875" t="s">
         <v>383</v>
@@ -16075,7 +16080,7 @@
     </row>
     <row r="876" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A876" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B876" s="1" t="s">
         <v>1540</v>
@@ -16086,7 +16091,7 @@
     </row>
     <row r="877" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A877" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B877" s="1" t="s">
         <v>1540</v>
@@ -16097,7 +16102,7 @@
     </row>
     <row r="878" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A878" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B878" s="1" t="s">
         <v>1540</v>
@@ -16108,7 +16113,7 @@
     </row>
     <row r="879" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A879" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B879" s="1" t="s">
         <v>1540</v>
@@ -16119,10 +16124,10 @@
     </row>
     <row r="880" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A880" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B880" s="1" t="s">
-        <v>1520</v>
+        <v>1540</v>
       </c>
       <c r="C880" t="s">
         <v>383</v>
@@ -16130,7 +16135,7 @@
     </row>
     <row r="881" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A881" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B881" s="1" t="s">
         <v>1520</v>
@@ -16141,7 +16146,7 @@
     </row>
     <row r="882" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A882" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B882" s="1" t="s">
         <v>1520</v>
@@ -16152,7 +16157,7 @@
     </row>
     <row r="883" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A883" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B883" s="1" t="s">
         <v>1520</v>
@@ -16163,7 +16168,7 @@
     </row>
     <row r="884" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A884" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B884" s="1" t="s">
         <v>1520</v>
@@ -16174,10 +16179,10 @@
     </row>
     <row r="885" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A885" s="1" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>1525</v>
+        <v>1520</v>
       </c>
       <c r="C885" t="s">
         <v>383</v>
@@ -16185,7 +16190,7 @@
     </row>
     <row r="886" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A886" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B886" s="1" t="s">
         <v>1525</v>
@@ -16196,7 +16201,7 @@
     </row>
     <row r="887" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A887" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B887" s="1" t="s">
         <v>1525</v>
@@ -16207,7 +16212,7 @@
     </row>
     <row r="888" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A888" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B888" s="1" t="s">
         <v>1525</v>
@@ -16218,7 +16223,7 @@
     </row>
     <row r="889" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A889" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B889" s="1" t="s">
         <v>1525</v>
@@ -16229,10 +16234,10 @@
     </row>
     <row r="890" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A890" s="1" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B890" s="1" t="s">
-        <v>1545</v>
+        <v>1525</v>
       </c>
       <c r="C890" t="s">
         <v>383</v>
@@ -16240,7 +16245,7 @@
     </row>
     <row r="891" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A891" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B891" s="1" t="s">
         <v>1545</v>
@@ -16251,7 +16256,7 @@
     </row>
     <row r="892" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A892" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B892" s="1" t="s">
         <v>1545</v>
@@ -16262,7 +16267,7 @@
     </row>
     <row r="893" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A893" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B893" s="1" t="s">
         <v>1545</v>
@@ -16273,7 +16278,7 @@
     </row>
     <row r="894" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A894" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B894" s="1" t="s">
         <v>1545</v>
@@ -16284,10 +16289,10 @@
     </row>
     <row r="895" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A895" s="1" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B895" s="1" t="s">
-        <v>1755</v>
+        <v>1545</v>
       </c>
       <c r="C895" t="s">
         <v>383</v>
@@ -16295,7 +16300,7 @@
     </row>
     <row r="896" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A896" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B896" s="1" t="s">
         <v>1755</v>
@@ -16306,7 +16311,7 @@
     </row>
     <row r="897" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A897" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B897" s="1" t="s">
         <v>1755</v>
@@ -16317,7 +16322,7 @@
     </row>
     <row r="898" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A898" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B898" s="1" t="s">
         <v>1755</v>
@@ -16328,7 +16333,7 @@
     </row>
     <row r="899" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A899" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B899" s="1" t="s">
         <v>1755</v>
@@ -16339,10 +16344,10 @@
     </row>
     <row r="900" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A900" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B900" s="1" t="s">
-        <v>1740</v>
+        <v>1755</v>
       </c>
       <c r="C900" t="s">
         <v>383</v>
@@ -16350,7 +16355,7 @@
     </row>
     <row r="901" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A901" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B901" s="1" t="s">
         <v>1740</v>
@@ -16361,7 +16366,7 @@
     </row>
     <row r="902" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A902" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B902" s="1" t="s">
         <v>1740</v>
@@ -16372,7 +16377,7 @@
     </row>
     <row r="903" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A903" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B903" s="1" t="s">
         <v>1740</v>
@@ -16383,7 +16388,7 @@
     </row>
     <row r="904" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A904" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B904" s="1" t="s">
         <v>1740</v>
@@ -16394,7 +16399,7 @@
     </row>
     <row r="905" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A905" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B905" s="1" t="s">
         <v>1740</v>
@@ -16405,10 +16410,10 @@
     </row>
     <row r="906" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A906" s="1" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="B906" s="1" t="s">
-        <v>1755</v>
+        <v>1740</v>
       </c>
       <c r="C906" t="s">
         <v>383</v>
@@ -16416,7 +16421,7 @@
     </row>
     <row r="907" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A907" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B907" s="1" t="s">
         <v>1755</v>
@@ -16427,7 +16432,7 @@
     </row>
     <row r="908" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A908" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B908" s="1" t="s">
         <v>1755</v>
@@ -16438,7 +16443,7 @@
     </row>
     <row r="909" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A909" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B909" s="1" t="s">
         <v>1755</v>
@@ -16449,7 +16454,7 @@
     </row>
     <row r="910" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A910" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B910" s="1" t="s">
         <v>1755</v>
@@ -16460,7 +16465,7 @@
     </row>
     <row r="911" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A911" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B911" s="1" t="s">
         <v>1755</v>
@@ -16471,10 +16476,10 @@
     </row>
     <row r="912" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A912" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B912" s="1" t="s">
-        <v>1520</v>
+        <v>1755</v>
       </c>
       <c r="C912" t="s">
         <v>383</v>
@@ -16482,7 +16487,7 @@
     </row>
     <row r="913" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A913" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B913" s="1" t="s">
         <v>1520</v>
@@ -16493,7 +16498,7 @@
     </row>
     <row r="914" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A914" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B914" s="1" t="s">
         <v>1520</v>
@@ -16504,7 +16509,7 @@
     </row>
     <row r="915" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A915" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B915" s="1" t="s">
         <v>1520</v>
@@ -16515,7 +16520,7 @@
     </row>
     <row r="916" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A916" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B916" s="1" t="s">
         <v>1520</v>
@@ -16525,11 +16530,11 @@
       </c>
     </row>
     <row r="917" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A917" s="1">
-        <v>1</v>
-      </c>
-      <c r="B917" t="s">
-        <v>1530</v>
+      <c r="A917" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B917" s="1" t="s">
+        <v>1520</v>
       </c>
       <c r="C917" t="s">
         <v>383</v>
@@ -16540,7 +16545,7 @@
         <v>1</v>
       </c>
       <c r="B918" t="s">
-        <v>1565</v>
+        <v>1530</v>
       </c>
       <c r="C918" t="s">
         <v>383</v>
@@ -16551,18 +16556,18 @@
         <v>1</v>
       </c>
       <c r="B919" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C919" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="920" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A920" s="1">
+        <v>1</v>
+      </c>
+      <c r="B920" t="s">
         <v>1896</v>
-      </c>
-      <c r="C919" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="920" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A920" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="B920" s="1" t="s">
-        <v>1760</v>
       </c>
       <c r="C920" t="s">
         <v>383</v>
@@ -16570,7 +16575,7 @@
     </row>
     <row r="921" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A921" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B921" s="1" t="s">
         <v>1760</v>
@@ -16581,7 +16586,7 @@
     </row>
     <row r="922" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A922" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B922" s="1" t="s">
         <v>1760</v>
@@ -16592,7 +16597,7 @@
     </row>
     <row r="923" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A923" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B923" s="1" t="s">
         <v>1760</v>
@@ -16603,7 +16608,7 @@
     </row>
     <row r="924" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A924" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B924" s="1" t="s">
         <v>1760</v>
@@ -16614,7 +16619,7 @@
     </row>
     <row r="925" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A925" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B925" s="1" t="s">
         <v>1760</v>
@@ -16625,7 +16630,7 @@
     </row>
     <row r="926" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A926" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B926" s="1" t="s">
         <v>1760</v>
@@ -16636,10 +16641,10 @@
     </row>
     <row r="927" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A927" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B927" s="1" t="s">
-        <v>1720</v>
+        <v>1760</v>
       </c>
       <c r="C927" t="s">
         <v>383</v>
@@ -16647,7 +16652,7 @@
     </row>
     <row r="928" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A928" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B928" s="1" t="s">
         <v>1720</v>
@@ -16658,7 +16663,7 @@
     </row>
     <row r="929" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A929" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B929" s="1" t="s">
         <v>1720</v>
@@ -16669,7 +16674,7 @@
     </row>
     <row r="930" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A930" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B930" s="1" t="s">
         <v>1720</v>
@@ -16680,7 +16685,7 @@
     </row>
     <row r="931" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A931" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B931" s="1" t="s">
         <v>1720</v>
@@ -16691,10 +16696,10 @@
     </row>
     <row r="932" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A932" s="1" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B932" s="1" t="s">
-        <v>1730</v>
+        <v>1720</v>
       </c>
       <c r="C932" t="s">
         <v>383</v>
@@ -16702,7 +16707,7 @@
     </row>
     <row r="933" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A933" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B933" s="1" t="s">
         <v>1730</v>
@@ -16713,7 +16718,7 @@
     </row>
     <row r="934" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A934" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B934" s="1" t="s">
         <v>1730</v>
@@ -16724,7 +16729,7 @@
     </row>
     <row r="935" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A935" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B935" s="1" t="s">
         <v>1730</v>
@@ -16735,7 +16740,7 @@
     </row>
     <row r="936" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A936" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B936" s="1" t="s">
         <v>1730</v>
@@ -16746,10 +16751,10 @@
     </row>
     <row r="937" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A937" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B937" s="1" t="s">
-        <v>1710</v>
+        <v>1730</v>
       </c>
       <c r="C937" t="s">
         <v>383</v>
@@ -16757,7 +16762,7 @@
     </row>
     <row r="938" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A938" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B938" s="1" t="s">
         <v>1710</v>
@@ -16768,7 +16773,7 @@
     </row>
     <row r="939" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A939" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B939" s="1" t="s">
         <v>1710</v>
@@ -16779,7 +16784,7 @@
     </row>
     <row r="940" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A940" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B940" s="1" t="s">
         <v>1710</v>
@@ -16790,7 +16795,7 @@
     </row>
     <row r="941" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A941" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B941" s="1" t="s">
         <v>1710</v>
@@ -16801,7 +16806,7 @@
     </row>
     <row r="942" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A942" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B942" s="1" t="s">
         <v>1710</v>
@@ -16812,10 +16817,10 @@
     </row>
     <row r="943" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A943" s="1" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="B943" s="1" t="s">
-        <v>1715</v>
+        <v>1710</v>
       </c>
       <c r="C943" t="s">
         <v>383</v>
@@ -16823,7 +16828,7 @@
     </row>
     <row r="944" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A944" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B944" s="1" t="s">
         <v>1715</v>
@@ -16834,7 +16839,7 @@
     </row>
     <row r="945" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A945" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B945" s="1" t="s">
         <v>1715</v>
@@ -16845,7 +16850,7 @@
     </row>
     <row r="946" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A946" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B946" s="1" t="s">
         <v>1715</v>
@@ -16856,7 +16861,7 @@
     </row>
     <row r="947" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A947" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B947" s="1" t="s">
         <v>1715</v>
@@ -16867,7 +16872,7 @@
     </row>
     <row r="948" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A948" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B948" s="1" t="s">
         <v>1715</v>
@@ -16878,10 +16883,10 @@
     </row>
     <row r="949" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A949" s="1" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="B949" s="1" t="s">
-        <v>1725</v>
+        <v>1715</v>
       </c>
       <c r="C949" t="s">
         <v>383</v>
@@ -16889,7 +16894,7 @@
     </row>
     <row r="950" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A950" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B950" s="1" t="s">
         <v>1725</v>
@@ -16900,7 +16905,7 @@
     </row>
     <row r="951" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A951" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B951" s="1" t="s">
         <v>1725</v>
@@ -16911,7 +16916,7 @@
     </row>
     <row r="952" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A952" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B952" s="1" t="s">
         <v>1725</v>
@@ -16922,7 +16927,7 @@
     </row>
     <row r="953" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A953" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B953" s="1" t="s">
         <v>1725</v>
@@ -16933,12 +16938,23 @@
     </row>
     <row r="954" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A954" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B954" s="1" t="s">
         <v>1725</v>
       </c>
       <c r="C954" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="955" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A955" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B955" s="1" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C955" t="s">
         <v>383</v>
       </c>
     </row>
@@ -17046,8 +17062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F440"/>
   <sheetViews>
-    <sheetView topLeftCell="A383" workbookViewId="0">
-      <selection activeCell="A414" sqref="A414"/>
+    <sheetView topLeftCell="A245" workbookViewId="0">
+      <selection activeCell="A255" sqref="A255:A260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24264,6 +24280,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -24271,7 +24288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>